<commit_message>
Update Day 2 and 3
</commit_message>
<xml_diff>
--- a/1.5 R Data IO/de-DE/TSLA.xlsx
+++ b/1.5 R Data IO/de-DE/TSLA.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dm_78\Source\Repos\r_training\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dm_78\Source\Repos\r_train_2\1.5 R Data IO\de-DE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8BBFA1B-613A-4C16-BAA6-B2E74B45D05D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCE73B5-B3C8-4165-B0E1-199E12FBCBC4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TSLA_EN" sheetId="1" r:id="rId1"/>
+    <sheet name="S2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1771" uniqueCount="1459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1871" uniqueCount="1459">
   <si>
     <t>Date</t>
   </si>
@@ -4402,7 +4403,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5237,10 +5238,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -11066,4 +11069,359 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF22F1D5-BCA3-4407-A44F-0A7CDDBE1CB0}">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>